<commit_message>
Modification bureau Catia MES48V
</commit_message>
<xml_diff>
--- a/Catia/Bancs et prototypes/proto batterie/module standard 48v/travail_JAuburtin/Modèle Catia/Calculs dimensions double feuille.xlsx
+++ b/Catia/Bancs et prototypes/proto batterie/module standard 48v/travail_JAuburtin/Modèle Catia/Calculs dimensions double feuille.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Desktop\Mes dossiers\Centrale Lyon\EPSA\Batterie\conception\Modèle Catia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Desktop\Mes dossiers\Centrale Lyon\EPSA\Batterie\travail_JAuburtin\Modèle Catia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E14E0F-DFE4-4A82-8C55-13091A6EE2A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D3FD17-8959-4CAD-9885-C9D46B0D0E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C=7" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="86">
   <si>
     <t>Grandeurs variables</t>
   </si>
@@ -292,6 +292,9 @@
   </si>
   <si>
     <t>enf_plg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centrer avec l'épaisseur </t>
   </si>
 </sst>
 </file>
@@ -640,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -793,6 +796,9 @@
       </c>
       <c r="C18" s="3">
         <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1213,7 +1219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2D4400-38A5-4808-BA0B-DD0884D9FFF0}">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Ajout de modèles de connexions électriques et réparation des fichiers Catia
</commit_message>
<xml_diff>
--- a/Catia/Bancs et prototypes/proto batterie/module standard 48v/travail_JAuburtin/Modèle Catia/Calculs dimensions double feuille.xlsx
+++ b/Catia/Bancs et prototypes/proto batterie/module standard 48v/travail_JAuburtin/Modèle Catia/Calculs dimensions double feuille.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Desktop\Mes dossiers\Centrale Lyon\EPSA\Batterie\travail_JAuburtin\Modèle Catia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D3FD17-8959-4CAD-9885-C9D46B0D0E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC71092A-B7E4-4742-9B45-17F345068243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="93">
   <si>
     <t>Grandeurs variables</t>
   </si>
@@ -295,6 +295,27 @@
   </si>
   <si>
     <t xml:space="preserve">Centrer avec l'épaisseur </t>
+  </si>
+  <si>
+    <t>epsilon</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>h_c</t>
+  </si>
+  <si>
+    <t>e_c</t>
+  </si>
+  <si>
+    <t>l_c</t>
+  </si>
+  <si>
+    <t>d_c</t>
+  </si>
+  <si>
+    <t>Dépassement du carter</t>
   </si>
 </sst>
 </file>
@@ -641,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -826,7 +847,7 @@
         <v>8</v>
       </c>
       <c r="C22">
-        <f>CEILING(2*C14+(C12-1)*C21+2*C18+C8+2*C49+2*C17,1)</f>
+        <f>CEILING(2*C14+(C12-1)*C21+2*C18+C8+2*C50+2*C17,1)</f>
         <v>145</v>
       </c>
     </row>
@@ -838,7 +859,7 @@
         <v>7</v>
       </c>
       <c r="C23">
-        <f>(C13)*C20+C8*(C13+1)+2*C15+2*C64+2*C16+2*C18</f>
+        <f>(C13)*C20+C8*(C13+1)+2*C15+2*C65+2*C16+2*C18</f>
         <v>278</v>
       </c>
     </row>
@@ -901,7 +922,7 @@
         <v>21</v>
       </c>
       <c r="B32" t="s">
-        <v>22</v>
+        <v>89</v>
       </c>
       <c r="C32" s="3">
         <v>5</v>
@@ -911,6 +932,9 @@
       <c r="A33" t="s">
         <v>19</v>
       </c>
+      <c r="B33" t="s">
+        <v>90</v>
+      </c>
       <c r="C33">
         <f>C22-2*C18+2*C32</f>
         <v>149</v>
@@ -948,267 +972,285 @@
         <v>25</v>
       </c>
       <c r="B37" t="s">
-        <v>26</v>
-      </c>
-      <c r="C37" s="3">
-        <v>25</v>
+        <v>88</v>
+      </c>
+      <c r="C37" s="2">
+        <f>C32+C40+C26+C38</f>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C38" s="3"/>
+      <c r="A38" t="s">
+        <v>92</v>
+      </c>
+      <c r="B38" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>30</v>
-      </c>
-      <c r="B39" t="s">
-        <v>31</v>
-      </c>
-      <c r="C39" s="3">
-        <v>4</v>
-      </c>
+      <c r="C39" s="2"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>35</v>
-      </c>
-      <c r="C40">
-        <f>C37-C39-C30-C26</f>
-        <v>13</v>
+        <v>30</v>
+      </c>
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" s="2">
+        <f>C30+C41</f>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>47</v>
+        <v>35</v>
+      </c>
+      <c r="B41" t="s">
+        <v>86</v>
       </c>
       <c r="C41" s="3">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>48</v>
       </c>
-      <c r="C42">
+      <c r="C43">
         <f>C33-2*C32</f>
         <v>139</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>49</v>
       </c>
-      <c r="C43">
+      <c r="C44">
         <f>C34-2*C32</f>
         <v>278</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>50</v>
-      </c>
-      <c r="C44">
-        <f>C49+(C32-C49) + C42</f>
-        <v>144</v>
-      </c>
-    </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45">
+        <f>C50+(C32-C50) + C43</f>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>51</v>
       </c>
-      <c r="C45">
-        <f>C60+C32-C60+C43</f>
+      <c r="C46">
+        <f>C61+C32-C61+C44</f>
         <v>283</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>29</v>
-      </c>
-      <c r="B49" t="s">
-        <v>67</v>
-      </c>
-      <c r="C49" s="3">
-        <v>0.5</v>
-      </c>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="B50" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C50" s="3">
-        <v>1</v>
-      </c>
-      <c r="D50" t="s">
-        <v>32</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="B51" t="s">
-        <v>76</v>
-      </c>
-      <c r="C51">
-        <f>C23-2*C16-2*C64+2*C55-2*C18</f>
-        <v>268</v>
+        <v>74</v>
+      </c>
+      <c r="C51" s="3">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B52" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C52">
-        <f>C7-2*C30-2*C26+2*C50</f>
-        <v>51</v>
+        <f>C23-2*C16-2*C65+2*C56-2*C18</f>
+        <v>268</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>43</v>
+        <v>34</v>
+      </c>
+      <c r="B53" t="s">
+        <v>75</v>
       </c>
       <c r="C53">
-        <f>C51/2</f>
-        <v>134</v>
+        <f>C7-2*C30-2*C26+2*C51</f>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C54">
         <f>C52/2</f>
-        <v>25.5</v>
+        <v>134</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>44</v>
+      </c>
+      <c r="C55">
+        <f>C53/2</f>
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>83</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>84</v>
       </c>
-      <c r="C55" s="2">
-        <f>C50</f>
+      <c r="C56" s="2">
+        <f>C51</f>
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="4" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B57" s="4"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>40</v>
-      </c>
-      <c r="B59" t="s">
-        <v>78</v>
-      </c>
-      <c r="C59">
-        <f>C7-C30*2-2*C26+2*C63</f>
-        <v>53</v>
-      </c>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
+        <v>40</v>
+      </c>
+      <c r="B60" t="s">
+        <v>78</v>
+      </c>
+      <c r="C60">
+        <f>C7-C30*2-2*C26+2*C64</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>41</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>79</v>
       </c>
-      <c r="C60">
+      <c r="C61">
         <f>C22-2*C18</f>
         <v>139</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D61" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>45</v>
-      </c>
-      <c r="C61">
-        <f>C59/2</f>
-        <v>26.5</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C62">
         <f>C60/2</f>
-        <v>69.5</v>
+        <v>26.5</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>63</v>
-      </c>
-      <c r="B63" t="s">
-        <v>80</v>
-      </c>
-      <c r="C63" s="3">
-        <v>2</v>
+        <v>46</v>
+      </c>
+      <c r="C63">
+        <f>C61/2</f>
+        <v>69.5</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>80</v>
+      </c>
+      <c r="C64" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>42</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>66</v>
       </c>
-      <c r="C64" s="3">
+      <c r="C65" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="4" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B66" s="4"/>
-      <c r="C66" s="4"/>
-      <c r="D66" s="4"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>37</v>
       </c>
-      <c r="C68">
-        <f>2*C40+C7</f>
-        <v>91</v>
+      <c r="C69">
+        <f>2*C41+C7</f>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A66:D66"/>
+    <mergeCell ref="A67:D67"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A5:D5"/>
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A58:D58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>